<commit_message>
final updates and quick fixes
</commit_message>
<xml_diff>
--- a/Planning/planning_2017/data/treegarden_2017plots.xlsx
+++ b/Planning/planning_2017/data/treegarden_2017plots.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="169">
   <si>
     <t>id</t>
   </si>
@@ -246,9 +246,6 @@
     <t>SPIALB</t>
   </si>
   <si>
-    <t>4?</t>
-  </si>
-  <si>
     <t>SPIALB04_HF</t>
   </si>
   <si>
@@ -259,9 +256,6 @@
   </si>
   <si>
     <t>SPIALB05_GR</t>
-  </si>
-  <si>
-    <t>8?</t>
   </si>
   <si>
     <t>SPIALB05_WM</t>
@@ -857,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="J117" sqref="J117"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -892,7 +886,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2541,8 +2535,8 @@
       <c r="G58" t="s">
         <v>58</v>
       </c>
-      <c r="H58" t="s">
-        <v>72</v>
+      <c r="H58">
+        <v>4</v>
       </c>
       <c r="J58" t="s">
         <v>11</v>
@@ -2550,7 +2544,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B59" t="s">
         <v>15</v>
@@ -2579,7 +2573,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B60" t="s">
         <v>15</v>
@@ -2599,8 +2593,8 @@
       <c r="G60" t="s">
         <v>58</v>
       </c>
-      <c r="H60" t="s">
-        <v>72</v>
+      <c r="H60">
+        <v>4</v>
       </c>
       <c r="J60" t="s">
         <v>11</v>
@@ -2608,7 +2602,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B61" t="s">
         <v>15</v>
@@ -2637,7 +2631,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B62" t="s">
         <v>15</v>
@@ -2666,7 +2660,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B63" t="s">
         <v>15</v>
@@ -2695,7 +2689,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B64" t="s">
         <v>15</v>
@@ -2715,8 +2709,8 @@
       <c r="G64" t="s">
         <v>58</v>
       </c>
-      <c r="H64" t="s">
-        <v>77</v>
+      <c r="H64">
+        <v>8</v>
       </c>
       <c r="J64" t="s">
         <v>11</v>
@@ -2724,7 +2718,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B65">
         <v>5</v>
@@ -2753,7 +2747,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B66">
         <v>5</v>
@@ -2782,7 +2776,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B67">
         <v>4</v>
@@ -2802,8 +2796,8 @@
       <c r="G67" t="s">
         <v>58</v>
       </c>
-      <c r="H67" t="s">
-        <v>72</v>
+      <c r="H67">
+        <v>4</v>
       </c>
       <c r="J67" t="s">
         <v>11</v>
@@ -2811,7 +2805,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B68">
         <v>4</v>
@@ -2831,8 +2825,8 @@
       <c r="G68" t="s">
         <v>58</v>
       </c>
-      <c r="H68" t="s">
-        <v>72</v>
+      <c r="H68">
+        <v>4</v>
       </c>
       <c r="J68" t="s">
         <v>11</v>
@@ -2840,7 +2834,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B69" t="s">
         <v>15</v>
@@ -2860,8 +2854,8 @@
       <c r="G69" t="s">
         <v>58</v>
       </c>
-      <c r="H69" t="s">
-        <v>77</v>
+      <c r="H69">
+        <v>8</v>
       </c>
       <c r="J69" t="s">
         <v>11</v>
@@ -2869,7 +2863,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B70">
         <v>3</v>
@@ -2889,8 +2883,8 @@
       <c r="G70" t="s">
         <v>58</v>
       </c>
-      <c r="H70" t="s">
-        <v>72</v>
+      <c r="H70">
+        <v>4</v>
       </c>
       <c r="J70" t="s">
         <v>11</v>
@@ -2898,7 +2892,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B71" t="s">
         <v>15</v>
@@ -2927,13 +2921,13 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B72">
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D72" t="s">
         <v>17</v>
@@ -2956,13 +2950,13 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B73">
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D73" t="s">
         <v>17</v>
@@ -2985,13 +2979,13 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B74">
         <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D74" t="s">
         <v>17</v>
@@ -3014,13 +3008,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B75">
         <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D75" t="s">
         <v>17</v>
@@ -3043,13 +3037,13 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B76" t="s">
         <v>15</v>
       </c>
       <c r="C76" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D76" t="s">
         <v>17</v>
@@ -3072,13 +3066,13 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B77" t="s">
         <v>15</v>
       </c>
       <c r="C77" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D77" t="s">
         <v>17</v>
@@ -3101,13 +3095,13 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B78" t="s">
         <v>15</v>
       </c>
       <c r="C78" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D78" t="s">
         <v>17</v>
@@ -3130,13 +3124,13 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B79" t="s">
         <v>15</v>
       </c>
       <c r="C79" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D79" t="s">
         <v>17</v>
@@ -3159,13 +3153,13 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B80">
         <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D80" t="s">
         <v>10</v>
@@ -3188,13 +3182,13 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B81">
         <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D81" t="s">
         <v>10</v>
@@ -3217,13 +3211,13 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B82" t="s">
         <v>15</v>
       </c>
       <c r="C82" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D82" t="s">
         <v>26</v>
@@ -3246,13 +3240,13 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B83" t="s">
         <v>15</v>
       </c>
       <c r="C83" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D83" t="s">
         <v>26</v>
@@ -3275,13 +3269,13 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B84">
         <v>3</v>
       </c>
       <c r="C84" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D84" t="s">
         <v>14</v>
@@ -3304,13 +3298,13 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B85">
         <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D85" t="s">
         <v>14</v>
@@ -3333,13 +3327,13 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B86">
         <v>3</v>
       </c>
       <c r="C86" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D86" t="s">
         <v>14</v>
@@ -3362,13 +3356,13 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B87">
         <v>3</v>
       </c>
       <c r="C87" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D87" t="s">
         <v>14</v>
@@ -3391,13 +3385,13 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B88">
         <v>3</v>
       </c>
       <c r="C88" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D88" t="s">
         <v>14</v>
@@ -3420,13 +3414,13 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B89">
         <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D89" t="s">
         <v>14</v>
@@ -3449,13 +3443,13 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B90">
         <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D90" t="s">
         <v>14</v>
@@ -3478,13 +3472,13 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B91">
         <v>3</v>
       </c>
       <c r="C91" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D91" t="s">
         <v>14</v>
@@ -3507,13 +3501,13 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B92" t="s">
         <v>15</v>
       </c>
       <c r="C92" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D92" t="s">
         <v>10</v>
@@ -3536,13 +3530,13 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B93" t="s">
         <v>15</v>
       </c>
       <c r="C93" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D93" t="s">
         <v>10</v>
@@ -3565,13 +3559,13 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B94" t="s">
         <v>15</v>
       </c>
       <c r="C94" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D94" t="s">
         <v>17</v>
@@ -3594,13 +3588,13 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B95" t="s">
         <v>15</v>
       </c>
       <c r="C95" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D95" t="s">
         <v>17</v>
@@ -3623,13 +3617,13 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B96">
         <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D96" t="s">
         <v>14</v>
@@ -3652,13 +3646,13 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B97">
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D97" t="s">
         <v>17</v>
@@ -3681,13 +3675,13 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B98" t="s">
         <v>15</v>
       </c>
       <c r="C98" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D98" t="s">
         <v>10</v>
@@ -3710,13 +3704,13 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B99">
         <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D99" t="s">
         <v>26</v>
@@ -3739,13 +3733,13 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B100">
         <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D100" t="s">
         <v>14</v>
@@ -3768,13 +3762,13 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B101">
         <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D101" t="s">
         <v>17</v>
@@ -3797,13 +3791,13 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B102">
         <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D102" t="s">
         <v>10</v>
@@ -3826,13 +3820,13 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B103">
         <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D103" t="s">
         <v>10</v>
@@ -3844,7 +3838,7 @@
         <v>9</v>
       </c>
       <c r="I103" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J103" t="s">
         <v>21</v>
@@ -3852,13 +3846,13 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B104">
         <v>4</v>
       </c>
       <c r="C104" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D104" t="s">
         <v>10</v>
@@ -3870,7 +3864,7 @@
         <v>9</v>
       </c>
       <c r="I104" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J104" t="s">
         <v>11</v>
@@ -3878,13 +3872,13 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B105" t="s">
         <v>15</v>
       </c>
       <c r="C105" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D105" t="s">
         <v>10</v>
@@ -3896,7 +3890,7 @@
         <v>6</v>
       </c>
       <c r="I105" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J105" t="s">
         <v>11</v>
@@ -3904,7 +3898,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C106" t="s">
         <v>50</v>
@@ -3919,7 +3913,7 @@
         <v>10</v>
       </c>
       <c r="I106" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J106" t="s">
         <v>11</v>
@@ -3927,7 +3921,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C107" t="s">
         <v>50</v>
@@ -3942,7 +3936,7 @@
         <v>13</v>
       </c>
       <c r="I107" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J107" t="s">
         <v>11</v>
@@ -3950,7 +3944,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C108" t="s">
         <v>50</v>
@@ -3965,7 +3959,7 @@
         <v>13</v>
       </c>
       <c r="I108" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J108" t="s">
         <v>11</v>
@@ -3973,7 +3967,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C109" t="s">
         <v>50</v>
@@ -3988,7 +3982,7 @@
         <v>13</v>
       </c>
       <c r="I109" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J109" t="s">
         <v>11</v>
@@ -3996,7 +3990,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C110" t="s">
         <v>50</v>
@@ -4011,7 +4005,7 @@
         <v>7</v>
       </c>
       <c r="I110" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J110" t="s">
         <v>11</v>
@@ -4019,7 +4013,7 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B111">
         <v>4</v>
@@ -4037,7 +4031,7 @@
         <v>9</v>
       </c>
       <c r="I111" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J111" t="s">
         <v>11</v>
@@ -4045,7 +4039,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B112" t="s">
         <v>15</v>
@@ -4063,7 +4057,7 @@
         <v>5</v>
       </c>
       <c r="I112" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J112" t="s">
         <v>21</v>
@@ -4071,7 +4065,7 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B113">
         <v>4</v>
@@ -4086,10 +4080,10 @@
         <v>11</v>
       </c>
       <c r="I113" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J113" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
@@ -4112,7 +4106,7 @@
         <v>15</v>
       </c>
       <c r="I114" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J114" t="s">
         <v>11</v>
@@ -4120,7 +4114,7 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B115">
         <v>3</v>
@@ -4138,7 +4132,7 @@
         <v>10</v>
       </c>
       <c r="I115" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J115" t="s">
         <v>11</v>
@@ -4146,7 +4140,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B116">
         <v>3</v>
@@ -4164,7 +4158,7 @@
         <v>13</v>
       </c>
       <c r="I116" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J116" t="s">
         <v>11</v>
@@ -4172,7 +4166,7 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B117">
         <v>3</v>
@@ -4190,7 +4184,7 @@
         <v>10</v>
       </c>
       <c r="I117" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J117" t="s">
         <v>21</v>
@@ -4198,7 +4192,7 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B118">
         <v>3</v>
@@ -4216,7 +4210,7 @@
         <v>10</v>
       </c>
       <c r="I118" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J118" t="s">
         <v>11</v>
@@ -4224,7 +4218,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B119">
         <v>4</v>
@@ -4242,7 +4236,7 @@
         <v>8</v>
       </c>
       <c r="I119" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J119" t="s">
         <v>21</v>
@@ -4257,7 +4251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -4271,431 +4265,431 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" t="s">
         <v>125</v>
-      </c>
-      <c r="B2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
         <v>125</v>
-      </c>
-      <c r="B3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
         <v>125</v>
-      </c>
-      <c r="B4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C29" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B31" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" t="s">
+        <v>164</v>
+      </c>
+      <c r="D36" t="s">
         <v>165</v>
-      </c>
-      <c r="B36" t="s">
-        <v>126</v>
-      </c>
-      <c r="C36" t="s">
-        <v>166</v>
-      </c>
-      <c r="D36" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C37" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>163</v>
+      </c>
+      <c r="B38" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" t="s">
         <v>165</v>
-      </c>
-      <c r="B38" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" t="s">
-        <v>166</v>
-      </c>
-      <c r="D38" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B39" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C39" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding some metadata tabs!
</commit_message>
<xml_diff>
--- a/Planning/planning_2017/data/treegarden_2017plots.xlsx
+++ b/Planning/planning_2017/data/treegarden_2017plots.xlsx
@@ -1,34 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8420" yWindow="460" windowWidth="24960" windowHeight="13520" tabRatio="500"/>
+    <workbookView xWindow="8420" yWindow="460" windowWidth="24960" windowHeight="13520" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="treegarden_2017plots" sheetId="1" r:id="rId1"/>
     <sheet name="tags" sheetId="2" r:id="rId2"/>
+    <sheet name="meta" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="174">
   <si>
     <t>id</t>
   </si>
@@ -535,19 +531,67 @@
   </si>
   <si>
     <t>not sure which one in 6!</t>
+  </si>
+  <si>
+    <t>treegarden_2017plots.xlsx was written by Cat, includes column indicating if a tag needs to be made or not. The “tags” sheet indicates which individuals need tags and where to find them.</t>
+  </si>
+  <si>
+    <t>From email from Cat on 12 May 2017:</t>
+  </si>
+  <si>
+    <t>So the first tab is for all new plants that need tags…</t>
+  </si>
+  <si>
+    <t>the second tab is for any plants coming from the raised beds that need a tag or for any of the plants already in the common garden that are missing tags.</t>
+  </si>
+  <si>
+    <t>from data/treegarden_2017plots_README.txt:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -567,13 +611,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -629,7 +687,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -664,7 +722,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -841,7 +899,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -851,16 +909,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -889,7 +947,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -918,7 +976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -947,7 +1005,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -976,7 +1034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1005,7 +1063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1034,7 +1092,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1063,7 +1121,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1092,7 +1150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1121,7 +1179,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1150,7 +1208,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1179,7 +1237,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1208,7 +1266,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1237,7 +1295,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1266,7 +1324,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1295,7 +1353,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1324,7 +1382,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1353,7 +1411,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1382,7 +1440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1411,7 +1469,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1440,7 +1498,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1469,7 +1527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1498,7 +1556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1527,7 +1585,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1556,7 +1614,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1585,7 +1643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1614,7 +1672,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1643,7 +1701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1672,7 +1730,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1701,7 +1759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1730,7 +1788,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1759,7 +1817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -1788,7 +1846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -1817,7 +1875,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1846,7 +1904,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -1875,7 +1933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1904,7 +1962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -1933,7 +1991,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -1962,7 +2020,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -1991,7 +2049,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -2020,7 +2078,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -2049,7 +2107,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -2078,7 +2136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -2107,7 +2165,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -2136,7 +2194,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -2165,7 +2223,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -2194,7 +2252,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -2223,7 +2281,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -2252,7 +2310,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -2281,7 +2339,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -2310,7 +2368,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>61</v>
       </c>
@@ -2339,7 +2397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -2368,7 +2426,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -2397,7 +2455,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -2426,7 +2484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -2455,7 +2513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -2484,7 +2542,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -2513,7 +2571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -2542,7 +2600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -2571,7 +2629,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>73</v>
       </c>
@@ -2600,7 +2658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -2629,7 +2687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -2658,7 +2716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -2687,7 +2745,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -2716,7 +2774,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>76</v>
       </c>
@@ -2745,7 +2803,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>76</v>
       </c>
@@ -2774,7 +2832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>77</v>
       </c>
@@ -2803,7 +2861,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
         <v>78</v>
       </c>
@@ -2832,7 +2890,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -2861,7 +2919,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>80</v>
       </c>
@@ -2890,7 +2948,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>81</v>
       </c>
@@ -2919,7 +2977,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
         <v>82</v>
       </c>
@@ -2948,7 +3006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -2977,7 +3035,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -3006,7 +3064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -3035,7 +3093,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -3064,7 +3122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -3093,7 +3151,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -3122,7 +3180,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>84</v>
       </c>
@@ -3151,7 +3209,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -3180,7 +3238,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -3209,7 +3267,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -3238,7 +3296,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -3267,7 +3325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10">
       <c r="A84" t="s">
         <v>89</v>
       </c>
@@ -3296,7 +3354,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10">
       <c r="A85" t="s">
         <v>89</v>
       </c>
@@ -3325,7 +3383,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10">
       <c r="A86" t="s">
         <v>89</v>
       </c>
@@ -3354,7 +3412,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10">
       <c r="A87" t="s">
         <v>89</v>
       </c>
@@ -3383,7 +3441,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10">
       <c r="A88" t="s">
         <v>89</v>
       </c>
@@ -3412,7 +3470,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -3441,7 +3499,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -3470,7 +3528,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -3499,7 +3557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -3528,7 +3586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10">
       <c r="A93" t="s">
         <v>90</v>
       </c>
@@ -3557,7 +3615,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -3586,7 +3644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10">
       <c r="A95" t="s">
         <v>92</v>
       </c>
@@ -3615,7 +3673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10">
       <c r="A96" t="s">
         <v>93</v>
       </c>
@@ -3644,7 +3702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -3673,7 +3731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -3702,7 +3760,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -3731,7 +3789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -3760,7 +3818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -3789,7 +3847,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -3818,7 +3876,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -3844,7 +3902,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10">
       <c r="A104" t="s">
         <v>101</v>
       </c>
@@ -3870,7 +3928,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10">
       <c r="A105" t="s">
         <v>101</v>
       </c>
@@ -3896,7 +3954,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -3919,7 +3977,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -3942,7 +4000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -3965,7 +4023,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -3988,7 +4046,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10">
       <c r="A110" t="s">
         <v>107</v>
       </c>
@@ -4011,7 +4069,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -4037,7 +4095,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -4063,7 +4121,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -4086,7 +4144,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10">
       <c r="A114" t="s">
         <v>29</v>
       </c>
@@ -4112,7 +4170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10">
       <c r="A115" t="s">
         <v>115</v>
       </c>
@@ -4138,7 +4196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10">
       <c r="A116" t="s">
         <v>117</v>
       </c>
@@ -4164,7 +4222,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10">
       <c r="A117" t="s">
         <v>118</v>
       </c>
@@ -4190,7 +4248,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10">
       <c r="A118" t="s">
         <v>119</v>
       </c>
@@ -4216,7 +4274,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10">
       <c r="A119" t="s">
         <v>120</v>
       </c>
@@ -4244,6 +4302,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4255,12 +4318,12 @@
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4268,7 +4331,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -4279,7 +4342,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -4290,7 +4353,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -4301,7 +4364,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -4312,7 +4375,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -4323,7 +4386,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>130</v>
       </c>
@@ -4334,7 +4397,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -4345,7 +4408,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>133</v>
       </c>
@@ -4356,7 +4419,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -4367,7 +4430,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>135</v>
       </c>
@@ -4378,7 +4441,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -4389,7 +4452,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -4400,7 +4463,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -4411,7 +4474,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -4422,7 +4485,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>138</v>
       </c>
@@ -4433,7 +4496,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -4444,7 +4507,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>143</v>
       </c>
@@ -4455,7 +4518,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>144</v>
       </c>
@@ -4466,7 +4529,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>146</v>
       </c>
@@ -4477,7 +4540,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>147</v>
       </c>
@@ -4488,7 +4551,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>133</v>
       </c>
@@ -4499,7 +4562,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>149</v>
       </c>
@@ -4510,7 +4573,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>133</v>
       </c>
@@ -4521,7 +4584,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>150</v>
       </c>
@@ -4532,7 +4595,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -4543,7 +4606,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>151</v>
       </c>
@@ -4554,7 +4617,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>153</v>
       </c>
@@ -4565,7 +4628,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>154</v>
       </c>
@@ -4576,7 +4639,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>156</v>
       </c>
@@ -4587,7 +4650,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>157</v>
       </c>
@@ -4598,7 +4661,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>158</v>
       </c>
@@ -4609,7 +4672,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>159</v>
       </c>
@@ -4620,7 +4683,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>161</v>
       </c>
@@ -4631,7 +4694,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>162</v>
       </c>
@@ -4642,7 +4705,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>163</v>
       </c>
@@ -4656,7 +4719,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>166</v>
       </c>
@@ -4667,7 +4730,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>163</v>
       </c>
@@ -4681,7 +4744,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>143</v>
       </c>
@@ -4694,5 +4757,104 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>